<commit_message>
Correction warning + ajout liste a restock dans le mail
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2irs\Desktop\E5\RPA Expertise\Projet\AutomatisationGestionCommandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B303C8-13BD-4E4F-9F6D-5041D3066627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19C5CE4-9561-4512-99AA-8A4964D90892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>